<commit_message>
Updated and added links
</commit_message>
<xml_diff>
--- a/extras/sample-forms/more-options/Timed categories - more options.xlsx
+++ b/extras/sample-forms/more-options/Timed categories - more options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Field plug-ins by Max/In progress/timed-categories/extras/sample-forms/more-options/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FA4CB6-DCDD-394E-89DF-D2DFAD0C5856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77E249C-232E-CB4D-8849-4FBC7BDC1128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="520" windowWidth="28800" windowHeight="16620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2558,12 +2558,6 @@
     <t>timed_categories_more_options</t>
   </si>
   <si>
-    <t>&lt;p&gt;In this sample form, we will demonstrate some of the additional features of the timed-categories field plug-in. If you just want a quick example of what the field plug-in can do, check out the &lt;a href="" target="_blank"&gt;simple form&lt;/a&gt;.&lt;/p&gt;
-&lt;p&gt;Times in this field plug-in are extra long so you can take your time to learn more about them. None of them are required, so you can swipe/click to skip ahead.&lt;/p&gt;
-&lt;br&gt;
-&lt;p&gt;To learn more about the field plug-in, check out the &lt;a href="" target="_blank"&gt;readme&lt;/a&gt;. If you just want a quick example of what the field plug-in can do, check out the &lt;a href="" target="_blank"&gt;simple form&lt;/a&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>custom-timed-categories(duration=999)</t>
   </si>
   <si>
@@ -2615,6 +2609,10 @@
     <t>&lt;p&gt;You can have as many columns as you'd like. They can even be randomized, like other choice lists.&lt;/p&gt;
 &lt;code&gt;randomized(0, 1) custom-timed-categories(duration=999)&lt;/code&gt;
 &lt;p&gt;Select your favorite crop&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In this sample form, we will demonstrate some of the additional features of the timed-categories field plug-in.&lt;/p&gt;
+&lt;p&gt;Times in this field plug-in are extra long so you can take your time to learn more about them. None of them are required, so you can swipe/click to skip ahead.&lt;/p&gt;&lt;p&gt;To learn more about the field plug-in, check out the &lt;a href="https://github.com/surveycto/timed-categories/blob/main/README.md" target="_blank"&gt;readme&lt;/a&gt;. For the main sample form, check out the sample form &lt;a href="https://github.com/surveycto/timed-categories/tree/main/extras/sample-forms/sample-main" target="_blank"&gt;here&lt;/a&gt;, which you can learn more about in the readme.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -4320,10 +4318,10 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C16" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -5167,7 +5165,7 @@
       <c r="Y11" s="11"/>
       <c r="Z11" s="11"/>
     </row>
-    <row r="12" spans="1:26" ht="255">
+    <row r="12" spans="1:26" ht="272">
       <c r="A12" s="41" t="s">
         <v>27</v>
       </c>
@@ -5175,7 +5173,7 @@
         <v>374</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>398</v>
+        <v>411</v>
       </c>
       <c r="D12" s="43"/>
       <c r="E12" s="41"/>
@@ -5239,7 +5237,7 @@
         <v>377</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="9"/>
@@ -5275,12 +5273,12 @@
         <v>378</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G15" s="9"/>
       <c r="H15" s="12"/>
@@ -5311,12 +5309,12 @@
         <v>392</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="12"/>
@@ -5347,12 +5345,12 @@
         <v>389</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="12"/>
@@ -5383,12 +5381,12 @@
         <v>388</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D18" s="12"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="G18" s="9"/>
       <c r="H18" s="12"/>
@@ -5419,12 +5417,12 @@
         <v>395</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D19" s="12"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G19" s="9"/>
       <c r="H19" s="12"/>
@@ -5455,12 +5453,12 @@
         <v>391</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="12"/>
@@ -61138,7 +61136,7 @@
       </c>
       <c r="C2" s="10" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2109062056</v>
+        <v>2109062210</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>38</v>

</xml_diff>